<commit_message>
Change spelling in spreadsheet file
</commit_message>
<xml_diff>
--- a/xlsx_files/AA_Tests_Empirical_Variance.xlsx
+++ b/xlsx_files/AA_Tests_Empirical_Variance.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WongT\Desktop\Projects\AB_Testing_Udacity\ABT_project_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WongT\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0085F4A0-A092-4A86-B0F3-49F81C258F13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E05502-D696-43A0-8F15-6123FEB1A382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -156,7 +156,7 @@
     <t>Differences should follow a normal distribution</t>
   </si>
   <si>
-    <t>Emperical standard error is the standard deviation of the observed differences</t>
+    <t>Empirical standard error is the standard deviation of the observed differences</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Made notes about checking distribution of metric
Do it using multiple A/A tests by plotting the histogram of your metric
and checking if it's normal
</commit_message>
<xml_diff>
--- a/xlsx_files/AA_Tests_Empirical_Variance.xlsx
+++ b/xlsx_files/AA_Tests_Empirical_Variance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WongT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WongT\Desktop\MOOC courses\AB_Testing_Udacity\ABT_project_files\xlsx_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E05502-D696-43A0-8F15-6123FEB1A382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D184D5-3F5A-4AEF-ADFC-ACD84D0B65DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Group 1</t>
   </si>
@@ -123,9 +123,6 @@
     <t>2 - Estimate variance and calculate CI of your metric if this wasn't able to be done analytically (maybe due to a complicated variance formula)</t>
   </si>
   <si>
-    <t>This is done emprically above by computing the sample standard deviation of "diff". Analytically it is done through the pooled variance formula which results in a different variance estimate for each experiment.</t>
-  </si>
-  <si>
     <t>The analytic estimate also makes the assumption of a normal distribution for diff.</t>
   </si>
   <si>
@@ -157,6 +154,12 @@
   </si>
   <si>
     <t>Empirical standard error is the standard deviation of the observed differences</t>
+  </si>
+  <si>
+    <t>This is done empirically above by computing the sample standard deviation of "diff". Analytically it is done through the pooled variance formula which results in a different variance estimate for each experiment.</t>
+  </si>
+  <si>
+    <t>Can check the distribution of the metric (diff) by plotting histogram.</t>
   </si>
 </sst>
 </file>
@@ -562,8 +565,8 @@
   </sheetPr>
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -774,7 +777,7 @@
         <v>YES</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
@@ -806,7 +809,7 @@
         <v/>
       </c>
       <c r="I8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
@@ -838,7 +841,7 @@
         <v/>
       </c>
       <c r="I9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
@@ -870,7 +873,7 @@
         <v/>
       </c>
       <c r="I10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
@@ -902,7 +905,7 @@
         <v/>
       </c>
       <c r="I11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
@@ -934,7 +937,7 @@
         <v/>
       </c>
       <c r="I12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
@@ -966,7 +969,7 @@
         <v/>
       </c>
       <c r="I13" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
@@ -1087,7 +1090,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
@@ -2198,12 +2203,12 @@
     </row>
     <row r="65" spans="1:3" ht="12.75">
       <c r="A65" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.75">
       <c r="A66" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="12.75">
@@ -2211,18 +2216,18 @@
         <v>24</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="12.75">
       <c r="A69" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:3" ht="12.75">
       <c r="A70" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="10"/>

</xml_diff>

<commit_message>
Edit empirical confidence interval discussion
They can be computed for skewed distributions but still implicitly
assume that observations at the tails are rare and can be removed
first.
</commit_message>
<xml_diff>
--- a/xlsx_files/AA_Tests_Empirical_Variance.xlsx
+++ b/xlsx_files/AA_Tests_Empirical_Variance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WongT\Desktop\MOOC courses\AB_Testing_Udacity\ABT_project_files\xlsx_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D184D5-3F5A-4AEF-ADFC-ACD84D0B65DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D59B72-D312-4B61-93A4-A3DCF806E22D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,12 +129,6 @@
     <t>3 - Directly estimate a confidence interval</t>
   </si>
   <si>
-    <t>This is done by sorting your "diffs" in ascending order and getting rid of samples from each end until you're left with 95% of the total samples. This boundary "diff" values is the emperical CI for diff.</t>
-  </si>
-  <si>
-    <t>This method can be used if your sampling distribution does not follow a normal distribution.</t>
-  </si>
-  <si>
     <t>Run 20 experiments on 0.5% of traffic</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>Can check the distribution of the metric (diff) by plotting histogram.</t>
+  </si>
+  <si>
+    <t>This is done by sorting your "diffs" in ascending order and getting rid of samples from each end until you're left with 95% of the total samples. This boundary "diff" values is the empirical CI for diff.</t>
+  </si>
+  <si>
+    <t>This method can be used if your sampling distribution is skewed but still implicitly assumes that observations at the tails are rare</t>
   </si>
 </sst>
 </file>
@@ -565,8 +565,8 @@
   </sheetPr>
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -777,7 +777,7 @@
         <v>YES</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
@@ -809,7 +809,7 @@
         <v/>
       </c>
       <c r="I8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
@@ -841,7 +841,7 @@
         <v/>
       </c>
       <c r="I9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
@@ -873,7 +873,7 @@
         <v/>
       </c>
       <c r="I10" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
@@ -905,7 +905,7 @@
         <v/>
       </c>
       <c r="I11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
@@ -937,7 +937,7 @@
         <v/>
       </c>
       <c r="I12" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
@@ -969,7 +969,7 @@
         <v/>
       </c>
       <c r="I13" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
@@ -1091,7 +1091,7 @@
         <v/>
       </c>
       <c r="I17" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
@@ -2203,7 +2203,7 @@
     </row>
     <row r="65" spans="1:3" ht="12.75">
       <c r="A65" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.75">
@@ -2221,13 +2221,13 @@
     </row>
     <row r="69" spans="1:3" ht="12.75">
       <c r="A69" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:3" ht="12.75">
       <c r="A70" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="10"/>

</xml_diff>